<commit_message>
Correcciones en dicciopnario de datos y diagrama de clases
</commit_message>
<xml_diff>
--- a/Diccionario de datos.xlsx
+++ b/Diccionario de datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelvi\Downloads\Tareas\Segundo periodo\DAE\proyecto final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7436F032-96FE-4CDA-A0E0-042136FC13BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4013A21D-6E4C-4FA9-81DC-6D82C9D47FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{33209235-A772-498A-84FC-93C94246B51E}"/>
+    <workbookView xWindow="22944" yWindow="7188" windowWidth="23232" windowHeight="12432" xr2:uid="{33209235-A772-498A-84FC-93C94246B51E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="88">
   <si>
     <t>Fecha</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Indica si el cargo se paga “Fijo” o “Por hora”.</t>
   </si>
   <si>
-    <t>salario_tarifa</t>
-  </si>
-  <si>
     <t>Decimal</t>
   </si>
   <si>
@@ -152,24 +149,12 @@
     <t>Documento Único de Identidad (formato: 00000000-0).</t>
   </si>
   <si>
-    <t>cargo_id</t>
-  </si>
-  <si>
     <t>Identificador del cargo asignado (clave foránea).</t>
   </si>
   <si>
-    <t>tipo_contrato</t>
-  </si>
-  <si>
-    <t>Tipo de contrato del empleado (“Fijo” o “Por hora”).</t>
-  </si>
-  <si>
     <t>salario_base</t>
   </si>
   <si>
-    <t>Salario mensual o tarifa por hora según contrato.</t>
-  </si>
-  <si>
     <t>horas_extras</t>
   </si>
   <si>
@@ -203,12 +188,6 @@
     <t>Empleado al que corresponde el pago (clave foránea).</t>
   </si>
   <si>
-    <t>periodo</t>
-  </si>
-  <si>
-    <t>Mes y año del cálculo (Ej. “Octubre 2025”).</t>
-  </si>
-  <si>
     <t>dias_trabajados</t>
   </si>
   <si>
@@ -245,9 +224,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>USUARIO (opcional)</t>
-  </si>
-  <si>
     <t>id_usuario</t>
   </si>
   <si>
@@ -260,9 +236,6 @@
     <t>Nombre del usuario.</t>
   </si>
   <si>
-    <t>contrasena</t>
-  </si>
-  <si>
     <t>Contraseña cifrada para acceso.</t>
   </si>
   <si>
@@ -291,6 +264,42 @@
   </si>
   <si>
     <t>Llave foranea del Id del empleado</t>
+  </si>
+  <si>
+    <t>hora_entrada</t>
+  </si>
+  <si>
+    <t>hora_salida</t>
+  </si>
+  <si>
+    <t>hh:mm</t>
+  </si>
+  <si>
+    <t>Hora en la que se registro la entrada</t>
+  </si>
+  <si>
+    <t>Hora en la que se registro la salida</t>
+  </si>
+  <si>
+    <t>Identificador único del empleado.</t>
+  </si>
+  <si>
+    <t>USUARIO</t>
+  </si>
+  <si>
+    <t>periodo_inicio</t>
+  </si>
+  <si>
+    <t>periodo_fin</t>
+  </si>
+  <si>
+    <t>Mes y año de inicio del cálculo (Ej. “Octubre 2025”).</t>
+  </si>
+  <si>
+    <t>Mes y año de fin del cálculo (Ej. “Octubre 2025”).</t>
+  </si>
+  <si>
+    <t>contrasenia</t>
   </si>
 </sst>
 </file>
@@ -334,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -345,6 +354,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,86 +689,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{902FED28-0579-449A-9175-C29159763357}">
-  <dimension ref="B9:F46"/>
+  <dimension ref="B7:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B39" zoomScale="151" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="B36" zoomScale="151" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" customWidth="1"/>
-    <col min="4" max="4" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="57.44140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="57.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2">
+        <v>11</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="2">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="2">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>78</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
         <v>15</v>
@@ -770,10 +808,10 @@
         <v>25</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
         <v>1</v>
@@ -788,7 +826,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
@@ -805,7 +843,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
         <v>21</v>
@@ -820,7 +858,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
         <v>23</v>
@@ -835,7 +873,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
         <v>25</v>
@@ -850,27 +888,27 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="2" t="s">
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>9</v>
@@ -879,118 +917,118 @@
         <v>11</v>
       </c>
       <c r="F20" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="C21" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E21" s="2">
-        <v>150</v>
+        <v>11</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="2">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E23" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E24" s="2">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
+      </c>
+      <c r="E25" s="2">
+        <v>10</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>45</v>
+        <v>16</v>
+      </c>
+      <c r="E26" s="2">
+        <v>50</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E27" s="2">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>16</v>
@@ -999,195 +1037,194 @@
         <v>50</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C29" s="2" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="2">
-        <v>50</v>
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="C30" s="2" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E30" s="2">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="2">
+        <v>11</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31" s="2" t="s">
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="D32" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E32" s="2">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>11</v>
+        <v>84</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="E33" s="2">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E34" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="2">
-        <v>2</v>
+        <v>27</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="F37" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>9</v>
@@ -1196,13 +1233,13 @@
         <v>11</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>16</v>
@@ -1211,13 +1248,13 @@
         <v>50</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>16</v>
@@ -1226,13 +1263,13 @@
         <v>50</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>9</v>
@@ -1241,27 +1278,31 @@
         <v>11</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>